<commit_message>
add logger and timi.py
</commit_message>
<xml_diff>
--- a/ko_test_excel.xlsx
+++ b/ko_test_excel.xlsx
@@ -322,9 +322,9 @@
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>this line is written by main.py</t>
+          <t>newline</t>
         </is>
       </c>
     </row>

</xml_diff>